<commit_message>
Convert model to onnx
</commit_message>
<xml_diff>
--- a/api/files/Models Version.xlsx
+++ b/api/files/Models Version.xlsx
@@ -5,20 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUDIT CỦA LEE JONG SON\Tengroup\Window-Audit-pipeline\src\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUDIT CỦA LEE JONG SON\Tengroup\Window-Audit-pipeline\src\api\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA807970-D994-43AD-A985-9E53763477E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F73264-D34B-4877-82FA-4FE11E57D50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
@@ -28,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Phiên bản</t>
   </si>
@@ -154,18 +163,29 @@
   </si>
   <si>
     <t>Rank(0-1): Càng thấp càng xuất hiện nhiều kết quả detect, nhưng đi kèm với chất lượng chính xác thấp</t>
+  </si>
+  <si>
+    <t>AD_YL11s_Seg_1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -277,28 +297,29 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -583,7 +604,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,7 +713,7 @@
       <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="13" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="3"/>
@@ -719,8 +740,12 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -913,7 +938,7 @@
       <c r="C23" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>